<commit_message>
Grafico de comparação adicionado
</commit_message>
<xml_diff>
--- a/Results/Resultados_Cons_Água.xlsx
+++ b/Results/Resultados_Cons_Água.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,26 +439,6 @@
           <t>Consumo de água 60°C</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Am 07</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Am 04</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Am 08</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Am 03</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,43 +446,11 @@
           <t>Peso Inicial (g)</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>Fase (0d - 21d)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+21dias</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>+21dias</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>+21dias</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>+21dias</t>
         </is>
       </c>
     </row>
@@ -512,18 +460,6 @@
           <t>Peso (g)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4.7</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -531,18 +467,6 @@
           <t>Wc 21d [g/Ah]</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>40.094</v>
-      </c>
-      <c r="C5" t="n">
-        <v>40.596</v>
-      </c>
-      <c r="D5" t="n">
-        <v>20.049</v>
-      </c>
-      <c r="E5" t="n">
-        <v>63.575</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added graph comparation and statistic data for WC
</commit_message>
<xml_diff>
--- a/Results/Resultados_Cons_Água.xlsx
+++ b/Results/Resultados_Cons_Água.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,26 @@
           <t>Consumo de água 60°C</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Am 03</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Am 04</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Am 07</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Am 08</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -446,6 +466,18 @@
           <t>Peso Inicial (g)</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>0.777</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -453,6 +485,26 @@
           <t>Fase (0d - 21d)</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>+21dias</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+21dias</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>+21dias</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>+21dias</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -460,12 +512,36 @@
           <t>Peso (g)</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.762</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.776</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Wc 21d [g/Ah]</t>
         </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.483</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.218</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.002</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>